<commit_message>
Edit experiment, test for 1h
</commit_message>
<xml_diff>
--- a/experiments/online/E6/P2/plant_reaction_test.xlsx
+++ b/experiments/online/E6/P2/plant_reaction_test.xlsx
@@ -85,7 +85,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -153,13 +153,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -169,22 +206,31 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="21" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -356,9 +402,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -438,7 +484,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -465,10 +511,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -715,9 +761,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -995,7 +1041,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1022,10 +1068,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1267,7 +1313,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1311,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>45756.541666666664</v>
+        <v>45756.5625</v>
       </c>
       <c r="C2" s="3">
         <v>0.26865</v>
@@ -1340,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="6">
-        <v>45756.582638888889</v>
+        <v>45756.610416666670</v>
       </c>
       <c r="C3" s="5">
         <v>0.26865</v>
@@ -1369,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>45756.583333333336</v>
+        <v>45756.611111111109</v>
       </c>
       <c r="C4" s="5">
         <v>0.1393</v>
@@ -1398,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="8">
-        <v>45756.603472222225</v>
+        <v>45756.610416666670</v>
       </c>
       <c r="C5" s="5">
         <v>0.1393</v>
@@ -1426,8 +1472,8 @@
       <c r="A6" s="5">
         <v>0</v>
       </c>
-      <c r="B6" s="8">
-        <v>45756.604166666664</v>
+      <c r="B6" s="7">
+        <v>45756.652777777781</v>
       </c>
       <c r="C6" s="5">
         <v>0.26865</v>
@@ -1456,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="8">
-        <v>45756.624305555553</v>
+        <v>45756.652083333334</v>
       </c>
       <c r="C7" s="5">
         <v>0.26865</v>
@@ -1484,8 +1530,8 @@
       <c r="A8" s="5">
         <v>0</v>
       </c>
-      <c r="B8" s="8">
-        <v>45756.625</v>
+      <c r="B8" s="7">
+        <v>45756.694444444445</v>
       </c>
       <c r="C8" s="5">
         <v>0.1393</v>
@@ -1514,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="8">
-        <v>45756.666666666664</v>
+        <v>45756.75</v>
       </c>
       <c r="C9" s="5">
         <v>0.1393</v>
@@ -1537,6 +1583,17 @@
       <c r="I9" s="5">
         <v>1</v>
       </c>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>